<commit_message>
agregue validaciones de todos los reportes
</commit_message>
<xml_diff>
--- a/datos_de_entrada/compras_MegaTools.xlsx
+++ b/datos_de_entrada/compras_MegaTools.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignacioviera/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b0137f82ab71419a/Desktop/proyecto-automatizacion-reporte-de-compras/automatizacion-reporte-compras/datos_de_entrada/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4B5A7E-47B7-3A49-A715-1B214A489776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{5F4B5A7E-47B7-3A49-A715-1B214A489776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1229400-3A36-4EBF-A34E-7FEC4389BB1E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17140" xr2:uid="{2BDAECEC-9689-E84F-8B6C-5832111FDE10}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2BDAECEC-9689-E84F-8B6C-5832111FDE10}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,24 +38,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
-    <t xml:space="preserve">Fecha </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proovedor </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Producto </t>
-  </si>
-  <si>
     <t>Cantidad</t>
   </si>
   <si>
-    <t xml:space="preserve">Precio Unitario </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Precio Total </t>
-  </si>
-  <si>
     <t>Martillo de acero</t>
   </si>
   <si>
@@ -68,7 +53,22 @@
     <t>Llave inglesa</t>
   </si>
   <si>
-    <t xml:space="preserve">MegaTools </t>
+    <t>Proveedor</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>MegaTools</t>
+  </si>
+  <si>
+    <t>Producto</t>
+  </si>
+  <si>
+    <t>PrecioTotal</t>
+  </si>
+  <si>
+    <t>PrecioUnitario</t>
   </si>
 </sst>
 </file>
@@ -78,7 +78,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -136,8 +136,12 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -456,47 +460,47 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" customWidth="1"/>
     <col min="3" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" customWidth="1"/>
     <col min="6" max="6" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.75">
       <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>45789</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>40</v>
@@ -508,15 +512,15 @@
         <v>280</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>45791</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>30</v>
@@ -528,15 +532,15 @@
         <v>360</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>45792</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>20</v>
@@ -548,15 +552,15 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>45795</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <v>50</v>

</xml_diff>